<commit_message>
add new task on tasks file
</commit_message>
<xml_diff>
--- a/casos de uso/casosdeuso.xlsx
+++ b/casos de uso/casosdeuso.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LabTiny\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LabTiny\Desktop\producto2\repositorio\PRODUCT_DESIGN\casos de uso\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -302,14 +302,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -318,13 +324,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -643,7 +643,7 @@
   <dimension ref="B1:R35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,15 +656,15 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
       <c r="P2" t="s">
         <v>45</v>
       </c>
@@ -676,15 +676,15 @@
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
       <c r="P3" t="s">
         <v>55</v>
       </c>
@@ -696,15 +696,15 @@
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
       <c r="M4" t="s">
         <v>51</v>
       </c>
@@ -719,15 +719,15 @@
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
       <c r="M5" t="s">
         <v>52</v>
       </c>
@@ -742,15 +742,15 @@
       <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
       <c r="M6" t="s">
         <v>53</v>
       </c>
@@ -762,20 +762,20 @@
       </c>
     </row>
     <row r="7" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
       <c r="M7" t="s">
         <v>57</v>
       </c>
@@ -787,18 +787,18 @@
       </c>
     </row>
     <row r="8" spans="2:18" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="12"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="4">
         <v>1</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
       <c r="L8" t="s">
         <v>59</v>
       </c>
@@ -813,35 +813,35 @@
       </c>
     </row>
     <row r="9" spans="2:18" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="12"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="4">
         <v>2</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
       <c r="P9" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="10" spans="2:18" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="12"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="4">
         <v>3</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
       <c r="O10" t="s">
         <v>62</v>
       </c>
@@ -850,357 +850,380 @@
       </c>
     </row>
     <row r="11" spans="2:18" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="12"/>
+      <c r="B11" s="6"/>
       <c r="C11" s="4">
         <v>4</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
     </row>
     <row r="12" spans="2:18" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="12"/>
+      <c r="B12" s="6"/>
       <c r="C12" s="4">
         <v>5</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
     </row>
     <row r="13" spans="2:18" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="12"/>
+      <c r="B13" s="6"/>
       <c r="C13" s="4">
         <v>6</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
     </row>
     <row r="14" spans="2:18" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="12"/>
+      <c r="B14" s="6"/>
       <c r="C14" s="4">
         <v>7</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
     </row>
     <row r="15" spans="2:18" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="12"/>
+      <c r="B15" s="6"/>
       <c r="C15" s="4">
         <v>8</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
     </row>
     <row r="16" spans="2:18" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="12"/>
+      <c r="B16" s="6"/>
       <c r="C16" s="4">
         <v>9</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
     </row>
     <row r="17" spans="2:9" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="12"/>
+      <c r="B17" s="6"/>
       <c r="C17" s="4">
         <v>10</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
     </row>
     <row r="18" spans="2:9" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="12"/>
+      <c r="B18" s="6"/>
       <c r="C18" s="4">
         <v>11</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
     </row>
     <row r="19" spans="2:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="12"/>
-      <c r="C19" s="5">
+      <c r="B19" s="6"/>
+      <c r="C19" s="12">
         <v>12</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
     </row>
     <row r="20" spans="2:9" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="12"/>
-      <c r="C20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="12"/>
       <c r="D20" s="4">
         <v>12.1</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
     </row>
     <row r="21" spans="2:9" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="12"/>
+      <c r="B21" s="6"/>
       <c r="C21" s="4">
         <v>13</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
     </row>
     <row r="22" spans="2:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="12"/>
+      <c r="B22" s="6"/>
       <c r="C22" s="4">
         <v>14</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
     </row>
     <row r="23" spans="2:9" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="12"/>
-      <c r="C23" s="5">
+      <c r="B23" s="6"/>
+      <c r="C23" s="12">
         <v>15</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
     </row>
     <row r="24" spans="2:9" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="12"/>
-      <c r="C24" s="5"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="12"/>
       <c r="D24" s="4">
         <v>15.1</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
     </row>
     <row r="25" spans="2:9" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="12"/>
+      <c r="B25" s="6"/>
       <c r="C25" s="4">
         <v>16</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
     </row>
     <row r="26" spans="2:9" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="12"/>
+      <c r="B26" s="6"/>
       <c r="C26" s="4">
         <v>17</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
     </row>
     <row r="27" spans="2:9" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="12"/>
+      <c r="B27" s="6"/>
       <c r="C27" s="4">
         <v>18</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
     </row>
     <row r="28" spans="2:9" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
     </row>
     <row r="29" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
     </row>
     <row r="30" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="5"/>
-      <c r="C30" s="5">
+      <c r="B30" s="12"/>
+      <c r="C30" s="12">
         <v>1</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
     </row>
     <row r="31" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
       <c r="D31" s="4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="E31" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
     </row>
     <row r="32" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
       <c r="D32" s="4">
         <v>1.2</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="E32" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
     </row>
     <row r="33" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
       <c r="D33" s="4">
         <v>1.3</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="E33" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
     </row>
     <row r="34" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
       <c r="D34" s="4">
         <v>1.4</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="E34" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
     </row>
     <row r="35" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="C35:I35"/>
+    <mergeCell ref="D27:I27"/>
+    <mergeCell ref="C28:I28"/>
+    <mergeCell ref="C30:C34"/>
+    <mergeCell ref="B29:B34"/>
+    <mergeCell ref="D29:I29"/>
+    <mergeCell ref="D30:I30"/>
+    <mergeCell ref="E31:I31"/>
+    <mergeCell ref="E32:I32"/>
+    <mergeCell ref="E33:I33"/>
+    <mergeCell ref="E34:I34"/>
+    <mergeCell ref="D26:I26"/>
+    <mergeCell ref="D17:I17"/>
+    <mergeCell ref="D18:I18"/>
+    <mergeCell ref="D19:I19"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="D21:I21"/>
+    <mergeCell ref="D22:I22"/>
+    <mergeCell ref="D23:I23"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="D25:I25"/>
     <mergeCell ref="C2:I2"/>
     <mergeCell ref="B7:B27"/>
     <mergeCell ref="D7:I7"/>
@@ -1217,29 +1240,6 @@
     <mergeCell ref="D13:I13"/>
     <mergeCell ref="D14:I14"/>
     <mergeCell ref="D15:I15"/>
-    <mergeCell ref="D26:I26"/>
-    <mergeCell ref="D17:I17"/>
-    <mergeCell ref="D18:I18"/>
-    <mergeCell ref="D19:I19"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="D21:I21"/>
-    <mergeCell ref="D22:I22"/>
-    <mergeCell ref="D23:I23"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="D25:I25"/>
-    <mergeCell ref="C35:I35"/>
-    <mergeCell ref="D27:I27"/>
-    <mergeCell ref="C28:I28"/>
-    <mergeCell ref="C30:C34"/>
-    <mergeCell ref="B29:B34"/>
-    <mergeCell ref="D29:I29"/>
-    <mergeCell ref="D30:I30"/>
-    <mergeCell ref="E31:I31"/>
-    <mergeCell ref="E32:I32"/>
-    <mergeCell ref="E33:I33"/>
-    <mergeCell ref="E34:I34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>